<commit_message>
Finished the smells analyze file.
</commit_message>
<xml_diff>
--- a/smells_analyze.xlsx
+++ b/smells_analyze.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\94848\git\csci3130\group\group16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E18E11-58C7-45E3-9977-23CBF608B831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AE466F-2788-4A4A-AED2-16D142030575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>File name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t xml:space="preserve">Refactored </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebSecurityConfig.java</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checking the sercurity authetic heeaders in every .authetic request.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -131,11 +143,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -424,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -436,121 +445,131 @@
     <col min="4" max="4" width="37.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="136" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="136" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="135.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="135.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="135.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="135.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="98" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="98" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="126" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="126" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>